<commit_message>
Add automatic publist, add matomo
</commit_message>
<xml_diff>
--- a/files/publist.xlsx
+++ b/files/publist.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Websites/Nicenet/Nicenet 2025 Quarto/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA8E364-C445-7149-B213-3045D6A30410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32135B1E-1D7B-9D42-A45F-1CA3A7E71688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="39260" windowHeight="22680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="39260" windowHeight="22680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Published" sheetId="1" r:id="rId1"/>
+    <sheet name="Preprints" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="322">
   <si>
     <t>doi</t>
   </si>
@@ -974,13 +975,25 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.31234/osf.io/4u8kj_v1</t>
+  </si>
+  <si>
+    <t>Interpersonal versus intrapersonal emotion regulation: Intensity of negative emotion predicts usage probability</t>
+  </si>
+  <si>
+    <t>https://osf.io/hjzpw/</t>
+  </si>
+  <si>
+    <t>https://osf.io/dwnya</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -992,6 +1005,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1014,16 +1035,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1328,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2866,4 +2890,81 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692218B6-AC24-C04C-84F2-434F3CE1F2AE}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="91.83203125" customWidth="1"/>
+    <col min="5" max="5" width="41.83203125" customWidth="1"/>
+    <col min="6" max="6" width="57.83203125" customWidth="1"/>
+    <col min="7" max="7" width="53.83203125" customWidth="1"/>
+    <col min="8" max="8" width="36.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2">
+        <v>2025</v>
+      </c>
+      <c r="C2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="G2" t="s">
+        <v>320</v>
+      </c>
+      <c r="H2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C2330C95-FE54-6C49-89D4-F219B0DEB161}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{5C49B39C-6DE3-8D44-AC9A-C79DEDEC6B41}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add VW grant; minor design tweaks
</commit_message>
<xml_diff>
--- a/files/publist.xlsx
+++ b/files/publist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Websites/Nicenet/Nicenet 2025 Quarto/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32135B1E-1D7B-9D42-A45F-1CA3A7E71688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879CDB53-4748-C341-B3B9-670561B98080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="39260" windowHeight="22680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="39260" windowHeight="22680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Published" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>https://osf.io/preprints/psyarxiv/jdh9m</t>
   </si>
   <si>
-    <t>https://doi.org/10.5160/psychdata.zrce%2016dy99_v20100</t>
-  </si>
-  <si>
     <t>https://osf.io/psqx8/</t>
   </si>
   <si>
@@ -987,6 +984,9 @@
   </si>
   <si>
     <t>https://osf.io/dwnya</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5160/psychdata.zrce16dy99_v20100</t>
   </si>
 </sst>
 </file>
@@ -1352,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1373,13 +1373,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1396,73 +1396,73 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B5">
         <v>2021</v>
       </c>
       <c r="C5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6">
         <v>2021</v>
       </c>
       <c r="C6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" t="s">
         <v>111</v>
-      </c>
-      <c r="E6" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B7">
         <v>2025</v>
       </c>
       <c r="C7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D7" t="s">
+        <v>312</v>
+      </c>
+      <c r="E7" t="s">
+        <v>311</v>
+      </c>
+      <c r="G7" t="s">
         <v>313</v>
-      </c>
-      <c r="E7" t="s">
-        <v>312</v>
-      </c>
-      <c r="G7" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B8">
         <v>2025</v>
       </c>
       <c r="C8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D8" t="s">
+        <v>309</v>
+      </c>
+      <c r="E8" t="s">
         <v>310</v>
-      </c>
-      <c r="E8" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1495,1399 +1495,1402 @@
       <c r="E10" t="s">
         <v>11</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="G10" t="s">
         <v>12</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>13</v>
-      </c>
-      <c r="H10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>2024</v>
       </c>
       <c r="C11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
         <v>16</v>
       </c>
-      <c r="E11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
         <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>2024</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>2023</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>2023</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>2023</v>
       </c>
       <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
         <v>26</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>27</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>28</v>
-      </c>
-      <c r="G15" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16">
         <v>2023</v>
       </c>
       <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
         <v>31</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>32</v>
-      </c>
-      <c r="G16" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17">
         <v>2023</v>
       </c>
       <c r="D17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
         <v>35</v>
-      </c>
-      <c r="E17" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>2023</v>
       </c>
       <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" t="s">
         <v>38</v>
-      </c>
-      <c r="E18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19">
         <v>2023</v>
       </c>
       <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" t="s">
         <v>41</v>
-      </c>
-      <c r="E19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20">
         <v>2022</v>
       </c>
       <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
         <v>44</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>45</v>
       </c>
-      <c r="F20" t="s">
-        <v>46</v>
-      </c>
       <c r="G20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21">
         <v>2022</v>
       </c>
       <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
         <v>48</v>
-      </c>
-      <c r="E21" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22">
         <v>2022</v>
       </c>
       <c r="D22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" t="s">
         <v>51</v>
-      </c>
-      <c r="E22" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23">
         <v>2022</v>
       </c>
       <c r="D23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s">
         <v>54</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>55</v>
-      </c>
-      <c r="G23" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24">
         <v>2022</v>
       </c>
       <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" t="s">
         <v>58</v>
-      </c>
-      <c r="E24" t="s">
-        <v>57</v>
-      </c>
-      <c r="G24" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25">
         <v>2022</v>
       </c>
       <c r="D25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" t="s">
         <v>61</v>
-      </c>
-      <c r="E25" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B26">
         <v>2022</v>
       </c>
       <c r="D26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" t="s">
         <v>64</v>
       </c>
-      <c r="E26" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" t="s">
         <v>65</v>
-      </c>
-      <c r="G26" t="s">
-        <v>65</v>
-      </c>
-      <c r="H26" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27">
         <v>2022</v>
       </c>
       <c r="D27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" t="s">
         <v>68</v>
       </c>
-      <c r="E27" t="s">
+      <c r="G27" t="s">
         <v>69</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>70</v>
-      </c>
-      <c r="H27" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B28">
         <v>2022</v>
       </c>
       <c r="D28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" t="s">
         <v>73</v>
       </c>
-      <c r="E28" t="s">
-        <v>72</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>74</v>
-      </c>
-      <c r="G28" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29">
         <v>2022</v>
       </c>
       <c r="D29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B30">
         <v>2022</v>
       </c>
       <c r="D30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31">
         <v>2022</v>
       </c>
       <c r="D31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" t="s">
         <v>81</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" t="s">
         <v>82</v>
-      </c>
-      <c r="G31" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32">
         <v>2022</v>
       </c>
       <c r="D32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" t="s">
         <v>85</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>86</v>
       </c>
-      <c r="F32" t="s">
-        <v>87</v>
-      </c>
       <c r="G32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B33">
         <v>2022</v>
       </c>
       <c r="D33" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" t="s">
         <v>89</v>
       </c>
-      <c r="E33" t="s">
+      <c r="G33" t="s">
         <v>90</v>
-      </c>
-      <c r="G33" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B34">
         <v>2022</v>
       </c>
       <c r="D34" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" t="s">
         <v>93</v>
       </c>
-      <c r="E34" t="s">
-        <v>92</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
+        <v>93</v>
+      </c>
+      <c r="H34" t="s">
         <v>94</v>
-      </c>
-      <c r="G34" t="s">
-        <v>94</v>
-      </c>
-      <c r="H34" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B35">
         <v>2021</v>
       </c>
       <c r="D35" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" t="s">
         <v>97</v>
       </c>
-      <c r="E35" t="s">
+      <c r="G35" t="s">
         <v>98</v>
-      </c>
-      <c r="G35" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B36">
         <v>2021</v>
       </c>
       <c r="D36" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" t="s">
         <v>101</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>102</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
+        <v>102</v>
+      </c>
+      <c r="H36" t="s">
         <v>103</v>
-      </c>
-      <c r="G36" t="s">
-        <v>103</v>
-      </c>
-      <c r="H36" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B37">
         <v>2021</v>
       </c>
       <c r="D37" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" t="s">
         <v>106</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>107</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>108</v>
-      </c>
-      <c r="G37" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B38">
         <v>2021</v>
       </c>
       <c r="D38" t="s">
+        <v>110</v>
+      </c>
+      <c r="E38" t="s">
         <v>111</v>
-      </c>
-      <c r="E38" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B39">
         <v>2021</v>
       </c>
       <c r="D39" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" t="s">
         <v>114</v>
-      </c>
-      <c r="E39" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B40">
         <v>2020</v>
       </c>
       <c r="D40" t="s">
+        <v>116</v>
+      </c>
+      <c r="E40" t="s">
         <v>117</v>
       </c>
-      <c r="E40" t="s">
+      <c r="G40" t="s">
         <v>118</v>
-      </c>
-      <c r="G40" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B41">
         <v>2020</v>
       </c>
       <c r="D41" t="s">
+        <v>120</v>
+      </c>
+      <c r="E41" t="s">
         <v>121</v>
-      </c>
-      <c r="E41" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B42">
         <v>2020</v>
       </c>
       <c r="D42" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42" t="s">
         <v>124</v>
       </c>
-      <c r="E42" t="s">
+      <c r="G42" t="s">
         <v>125</v>
-      </c>
-      <c r="G42" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B43">
         <v>2020</v>
       </c>
       <c r="D43" t="s">
+        <v>127</v>
+      </c>
+      <c r="E43" t="s">
         <v>128</v>
-      </c>
-      <c r="E43" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B44">
         <v>2020</v>
       </c>
       <c r="D44" t="s">
+        <v>130</v>
+      </c>
+      <c r="E44" t="s">
+        <v>129</v>
+      </c>
+      <c r="F44" t="s">
         <v>131</v>
       </c>
-      <c r="E44" t="s">
-        <v>130</v>
-      </c>
-      <c r="F44" t="s">
-        <v>132</v>
-      </c>
       <c r="G44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B45">
         <v>2020</v>
       </c>
       <c r="D45" t="s">
+        <v>133</v>
+      </c>
+      <c r="E45" t="s">
+        <v>132</v>
+      </c>
+      <c r="F45" t="s">
+        <v>73</v>
+      </c>
+      <c r="G45" t="s">
         <v>134</v>
       </c>
-      <c r="E45" t="s">
-        <v>133</v>
-      </c>
-      <c r="F45" t="s">
-        <v>74</v>
-      </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>135</v>
-      </c>
-      <c r="H45" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B46">
         <v>2020</v>
       </c>
       <c r="D46" t="s">
+        <v>137</v>
+      </c>
+      <c r="E46" t="s">
         <v>138</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>139</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>140</v>
-      </c>
-      <c r="G46" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B47">
         <v>2020</v>
       </c>
       <c r="D47" t="s">
+        <v>142</v>
+      </c>
+      <c r="E47" t="s">
         <v>143</v>
       </c>
-      <c r="E47" t="s">
+      <c r="G47" t="s">
         <v>144</v>
-      </c>
-      <c r="G47" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B48">
         <v>2019</v>
       </c>
       <c r="D48" t="s">
+        <v>146</v>
+      </c>
+      <c r="E48" t="s">
         <v>147</v>
       </c>
-      <c r="E48" t="s">
+      <c r="G48" t="s">
         <v>148</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>149</v>
-      </c>
-      <c r="H48" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B49">
         <v>2019</v>
       </c>
       <c r="D49" t="s">
+        <v>151</v>
+      </c>
+      <c r="E49" t="s">
         <v>152</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>153</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
+        <v>153</v>
+      </c>
+      <c r="H49" t="s">
         <v>154</v>
-      </c>
-      <c r="G49" t="s">
-        <v>154</v>
-      </c>
-      <c r="H49" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B50">
         <v>2019</v>
       </c>
       <c r="D50" t="s">
+        <v>156</v>
+      </c>
+      <c r="E50" t="s">
         <v>157</v>
-      </c>
-      <c r="E50" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B51">
         <v>2019</v>
       </c>
       <c r="D51" t="s">
+        <v>159</v>
+      </c>
+      <c r="E51" t="s">
         <v>160</v>
-      </c>
-      <c r="E51" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B52">
         <v>2019</v>
       </c>
       <c r="D52" t="s">
+        <v>162</v>
+      </c>
+      <c r="E52" t="s">
         <v>163</v>
       </c>
-      <c r="E52" t="s">
+      <c r="G52" t="s">
         <v>164</v>
-      </c>
-      <c r="G52" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B53">
         <v>2019</v>
       </c>
       <c r="D53" t="s">
+        <v>166</v>
+      </c>
+      <c r="E53" t="s">
         <v>167</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>168</v>
       </c>
-      <c r="F53" t="s">
-        <v>169</v>
-      </c>
       <c r="G53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B54">
         <v>2019</v>
       </c>
       <c r="D54" t="s">
+        <v>170</v>
+      </c>
+      <c r="E54" t="s">
         <v>171</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>172</v>
       </c>
-      <c r="F54" t="s">
-        <v>173</v>
-      </c>
       <c r="G54" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B55">
         <v>2019</v>
       </c>
       <c r="D55" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B56">
         <v>2019</v>
       </c>
       <c r="D56" t="s">
+        <v>176</v>
+      </c>
+      <c r="E56" t="s">
         <v>177</v>
       </c>
-      <c r="E56" t="s">
+      <c r="G56" t="s">
         <v>178</v>
-      </c>
-      <c r="G56" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B57">
         <v>2018</v>
       </c>
       <c r="D57" t="s">
+        <v>180</v>
+      </c>
+      <c r="E57" t="s">
         <v>181</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>182</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
+        <v>182</v>
+      </c>
+      <c r="H57" t="s">
         <v>183</v>
-      </c>
-      <c r="G57" t="s">
-        <v>183</v>
-      </c>
-      <c r="H57" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B58">
         <v>2018</v>
       </c>
       <c r="D58" t="s">
+        <v>185</v>
+      </c>
+      <c r="E58" t="s">
         <v>186</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>187</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
+        <v>187</v>
+      </c>
+      <c r="H58" t="s">
         <v>188</v>
-      </c>
-      <c r="G58" t="s">
-        <v>188</v>
-      </c>
-      <c r="H58" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B59">
         <v>2018</v>
       </c>
       <c r="D59" t="s">
+        <v>190</v>
+      </c>
+      <c r="E59" t="s">
         <v>191</v>
       </c>
-      <c r="E59" t="s">
+      <c r="G59" t="s">
         <v>192</v>
-      </c>
-      <c r="G59" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B60">
         <v>2018</v>
       </c>
       <c r="D60" t="s">
+        <v>194</v>
+      </c>
+      <c r="E60" t="s">
         <v>195</v>
       </c>
-      <c r="E60" t="s">
+      <c r="G60" t="s">
         <v>196</v>
-      </c>
-      <c r="G60" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B61">
         <v>2018</v>
       </c>
       <c r="D61" t="s">
+        <v>198</v>
+      </c>
+      <c r="E61" t="s">
         <v>199</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>200</v>
       </c>
-      <c r="F61" t="s">
-        <v>201</v>
-      </c>
       <c r="G61" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B62">
         <v>2018</v>
       </c>
       <c r="D62" t="s">
+        <v>202</v>
+      </c>
+      <c r="E62" t="s">
         <v>203</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>204</v>
       </c>
-      <c r="F62" t="s">
+      <c r="G62" t="s">
         <v>205</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>206</v>
-      </c>
-      <c r="H62" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B63">
         <v>2018</v>
       </c>
       <c r="D63" t="s">
+        <v>208</v>
+      </c>
+      <c r="E63" t="s">
         <v>209</v>
-      </c>
-      <c r="E63" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B64">
         <v>2017</v>
       </c>
       <c r="D64" t="s">
+        <v>211</v>
+      </c>
+      <c r="E64" t="s">
         <v>212</v>
-      </c>
-      <c r="E64" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B65">
         <v>2017</v>
       </c>
       <c r="D65" t="s">
+        <v>214</v>
+      </c>
+      <c r="E65" t="s">
         <v>215</v>
-      </c>
-      <c r="E65" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B66">
         <v>2017</v>
       </c>
       <c r="D66" t="s">
+        <v>217</v>
+      </c>
+      <c r="E66" t="s">
         <v>218</v>
-      </c>
-      <c r="E66" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B67">
         <v>2017</v>
       </c>
       <c r="D67" t="s">
+        <v>220</v>
+      </c>
+      <c r="E67" t="s">
         <v>221</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
         <v>222</v>
       </c>
-      <c r="F67" t="s">
-        <v>223</v>
-      </c>
       <c r="G67" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B68">
         <v>2017</v>
       </c>
       <c r="D68" t="s">
+        <v>224</v>
+      </c>
+      <c r="E68" t="s">
         <v>225</v>
       </c>
-      <c r="E68" t="s">
+      <c r="G68" t="s">
         <v>226</v>
-      </c>
-      <c r="G68" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B69">
         <v>2017</v>
       </c>
       <c r="D69" t="s">
+        <v>228</v>
+      </c>
+      <c r="E69" t="s">
         <v>229</v>
       </c>
-      <c r="E69" t="s">
+      <c r="F69" t="s">
         <v>230</v>
       </c>
-      <c r="F69" t="s">
-        <v>231</v>
-      </c>
       <c r="G69" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B70">
         <v>2017</v>
       </c>
       <c r="D70" t="s">
+        <v>232</v>
+      </c>
+      <c r="E70" t="s">
         <v>233</v>
-      </c>
-      <c r="E70" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B71">
         <v>2016</v>
       </c>
       <c r="C71" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D71" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E71" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B72">
         <v>2016</v>
       </c>
       <c r="D72" t="s">
+        <v>237</v>
+      </c>
+      <c r="E72" t="s">
         <v>238</v>
-      </c>
-      <c r="E72" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B73">
         <v>2016</v>
       </c>
       <c r="D73" t="s">
+        <v>240</v>
+      </c>
+      <c r="E73" t="s">
         <v>241</v>
-      </c>
-      <c r="E73" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B74">
         <v>2016</v>
       </c>
       <c r="D74" t="s">
+        <v>243</v>
+      </c>
+      <c r="E74" t="s">
         <v>244</v>
-      </c>
-      <c r="E74" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B75">
         <v>2016</v>
       </c>
       <c r="D75" t="s">
+        <v>246</v>
+      </c>
+      <c r="E75" t="s">
         <v>247</v>
-      </c>
-      <c r="E75" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B76">
         <v>2015</v>
       </c>
       <c r="D76" t="s">
+        <v>249</v>
+      </c>
+      <c r="E76" t="s">
         <v>250</v>
       </c>
-      <c r="E76" t="s">
+      <c r="G76" t="s">
         <v>251</v>
-      </c>
-      <c r="G76" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B77">
         <v>2015</v>
       </c>
       <c r="D77" t="s">
+        <v>253</v>
+      </c>
+      <c r="E77" t="s">
         <v>254</v>
-      </c>
-      <c r="E77" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B78">
         <v>2015</v>
       </c>
       <c r="D78" t="s">
+        <v>256</v>
+      </c>
+      <c r="E78" t="s">
         <v>257</v>
-      </c>
-      <c r="E78" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B79">
         <v>2015</v>
       </c>
       <c r="D79" t="s">
+        <v>259</v>
+      </c>
+      <c r="E79" t="s">
         <v>260</v>
-      </c>
-      <c r="E79" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B80">
         <v>2015</v>
       </c>
       <c r="D80" t="s">
+        <v>262</v>
+      </c>
+      <c r="E80" t="s">
         <v>263</v>
       </c>
-      <c r="E80" t="s">
+      <c r="G80" t="s">
         <v>264</v>
-      </c>
-      <c r="G80" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B81">
         <v>2015</v>
       </c>
       <c r="D81" t="s">
+        <v>266</v>
+      </c>
+      <c r="E81" t="s">
         <v>267</v>
-      </c>
-      <c r="E81" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B82">
         <v>2015</v>
       </c>
       <c r="D82" t="s">
+        <v>269</v>
+      </c>
+      <c r="E82" t="s">
         <v>270</v>
-      </c>
-      <c r="E82" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B83">
         <v>2014</v>
       </c>
       <c r="D83" t="s">
+        <v>272</v>
+      </c>
+      <c r="E83" t="s">
         <v>273</v>
       </c>
-      <c r="E83" t="s">
+      <c r="F83" t="s">
         <v>274</v>
       </c>
-      <c r="F83" t="s">
-        <v>275</v>
-      </c>
       <c r="G83" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B84">
         <v>2014</v>
       </c>
       <c r="D84" t="s">
+        <v>276</v>
+      </c>
+      <c r="E84" t="s">
         <v>277</v>
-      </c>
-      <c r="E84" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B85">
         <v>2014</v>
       </c>
       <c r="D85" t="s">
+        <v>279</v>
+      </c>
+      <c r="E85" t="s">
         <v>280</v>
-      </c>
-      <c r="E85" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B86">
         <v>2013</v>
       </c>
       <c r="D86" t="s">
+        <v>282</v>
+      </c>
+      <c r="E86" t="s">
         <v>283</v>
       </c>
-      <c r="E86" t="s">
+      <c r="G86" t="s">
         <v>284</v>
-      </c>
-      <c r="G86" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B87">
         <v>2012</v>
       </c>
       <c r="D87" t="s">
+        <v>286</v>
+      </c>
+      <c r="E87" t="s">
         <v>287</v>
-      </c>
-      <c r="E87" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B88">
         <v>2011</v>
       </c>
       <c r="D88" t="s">
+        <v>289</v>
+      </c>
+      <c r="E88" t="s">
         <v>290</v>
       </c>
-      <c r="E88" t="s">
+      <c r="G88" t="s">
         <v>291</v>
-      </c>
-      <c r="G88" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B89">
         <v>2011</v>
       </c>
       <c r="D89" t="s">
+        <v>293</v>
+      </c>
+      <c r="E89" t="s">
         <v>294</v>
-      </c>
-      <c r="E89" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B90">
         <v>2011</v>
       </c>
       <c r="D90" t="s">
+        <v>296</v>
+      </c>
+      <c r="E90" t="s">
         <v>297</v>
-      </c>
-      <c r="E90" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B91">
         <v>2011</v>
       </c>
       <c r="D91" t="s">
+        <v>299</v>
+      </c>
+      <c r="E91" t="s">
         <v>300</v>
-      </c>
-      <c r="E91" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B92">
         <v>2010</v>
       </c>
       <c r="D92" t="s">
+        <v>302</v>
+      </c>
+      <c r="E92" t="s">
         <v>303</v>
       </c>
-      <c r="E92" t="s">
-        <v>304</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F10" r:id="rId1" xr:uid="{57E6435F-936F-B049-820C-8B8D8672A77C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2896,7 +2899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692218B6-AC24-C04C-84F2-434F3CE1F2AE}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -2916,13 +2919,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -2939,25 +2942,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B2">
         <v>2025</v>
       </c>
       <c r="C2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G2" t="s">
         <v>319</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>320</v>
-      </c>
-      <c r="H2" t="s">
-        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add preprints to publication list
</commit_message>
<xml_diff>
--- a/files/publist.xlsx
+++ b/files/publist.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Websites/Nicenet/Nicenet 2025 Quarto/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879CDB53-4748-C341-B3B9-670561B98080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D02A6D-80DD-9C4F-88E5-3142C301375F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="39260" windowHeight="22680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4960" yWindow="760" windowWidth="34420" windowHeight="21280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Published" sheetId="1" r:id="rId1"/>
     <sheet name="Preprints" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Published!$A$1:$H$1</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="324">
   <si>
     <t>doi</t>
   </si>
@@ -987,6 +990,12 @@
   </si>
   <si>
     <t>https://doi.org/10.5160/psychdata.zrce16dy99_v20100</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.15626/MP.2023.3688</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1037/emo0001508</t>
   </si>
 </sst>
 </file>
@@ -1350,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H92"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1394,1502 +1403,1512 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B3">
+        <v>2025</v>
+      </c>
+      <c r="D3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G3" t="s">
+        <v>319</v>
+      </c>
+      <c r="H3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B4">
+        <v>2021</v>
+      </c>
+      <c r="C4" t="s">
+        <v>306</v>
+      </c>
+      <c r="D4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E4" t="s">
+        <v>314</v>
+      </c>
+    </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B5">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="C5" t="s">
         <v>306</v>
       </c>
       <c r="D5" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E5" t="s">
-        <v>314</v>
+        <v>311</v>
+      </c>
+      <c r="G5" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>308</v>
       </c>
       <c r="B6">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="C6" t="s">
         <v>306</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>309</v>
       </c>
       <c r="E6" t="s">
-        <v>111</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>311</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>2025</v>
       </c>
-      <c r="C7" t="s">
-        <v>306</v>
-      </c>
       <c r="D7" t="s">
-        <v>312</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>311</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>313</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>308</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>2025</v>
-      </c>
-      <c r="C8" t="s">
-        <v>306</v>
+        <v>2024</v>
       </c>
       <c r="D8" t="s">
-        <v>309</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>310</v>
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>2025</v>
+        <v>2024</v>
+      </c>
+      <c r="C9" t="s">
+        <v>306</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>2024</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B11">
-        <v>2024</v>
-      </c>
-      <c r="C11" t="s">
-        <v>306</v>
+        <v>2023</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B12">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>2023</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B14">
         <v>2023</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>31</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>2023</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B16">
         <v>2023</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G16" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B17">
         <v>2023</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B18">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
+        <v>45</v>
       </c>
       <c r="G18" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B19">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B20">
         <v>2022</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B21">
         <v>2022</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="G21" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>49</v>
+      <c r="A22" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="B22">
-        <v>2022</v>
+        <v>2025</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
+        <v>56</v>
+      </c>
+      <c r="G22" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B23">
         <v>2022</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>307</v>
       </c>
       <c r="B24">
         <v>2022</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>62</v>
+      </c>
+      <c r="F24" t="s">
+        <v>64</v>
       </c>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="H24" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B25">
         <v>2022</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>68</v>
+      </c>
+      <c r="G25" t="s">
+        <v>69</v>
+      </c>
+      <c r="H25" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>307</v>
+        <v>71</v>
       </c>
       <c r="B26">
         <v>2022</v>
       </c>
       <c r="D26" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F26" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="G26" t="s">
-        <v>64</v>
-      </c>
-      <c r="H26" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B27">
         <v>2022</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>68</v>
-      </c>
-      <c r="G27" t="s">
-        <v>69</v>
-      </c>
-      <c r="H27" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B28">
         <v>2022</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" t="s">
-        <v>73</v>
-      </c>
-      <c r="G28" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B29">
         <v>2022</v>
       </c>
       <c r="D29" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E29" t="s">
-        <v>75</v>
+        <v>81</v>
+      </c>
+      <c r="G29" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B30">
         <v>2022</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E30" t="s">
-        <v>77</v>
+        <v>85</v>
+      </c>
+      <c r="F30" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B31">
         <v>2022</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E31" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="G31" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B32">
         <v>2022</v>
       </c>
       <c r="D32" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F32" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G32" t="s">
-        <v>86</v>
+        <v>93</v>
+      </c>
+      <c r="H32" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B33">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="E33" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="G33" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B34">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D34" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E34" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="F34" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="G34" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="H34" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B35">
         <v>2021</v>
       </c>
       <c r="D35" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="E35" t="s">
-        <v>97</v>
+        <v>106</v>
+      </c>
+      <c r="F35" t="s">
+        <v>107</v>
       </c>
       <c r="G35" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B36">
         <v>2021</v>
       </c>
+      <c r="C36" t="s">
+        <v>306</v>
+      </c>
       <c r="D36" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E36" t="s">
-        <v>101</v>
-      </c>
-      <c r="F36" t="s">
-        <v>102</v>
-      </c>
-      <c r="G36" t="s">
-        <v>102</v>
-      </c>
-      <c r="H36" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B37">
         <v>2021</v>
       </c>
       <c r="D37" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E37" t="s">
-        <v>106</v>
-      </c>
-      <c r="F37" t="s">
-        <v>107</v>
-      </c>
-      <c r="G37" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B38">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D38" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E38" t="s">
-        <v>111</v>
+        <v>117</v>
+      </c>
+      <c r="G38" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B39">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D39" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="E39" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B40">
         <v>2020</v>
       </c>
       <c r="D40" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E40" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="G40" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B41">
         <v>2020</v>
       </c>
       <c r="D41" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="E41" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B42">
         <v>2020</v>
       </c>
       <c r="D42" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="E42" t="s">
-        <v>124</v>
+        <v>129</v>
+      </c>
+      <c r="F42" t="s">
+        <v>131</v>
       </c>
       <c r="G42" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B43">
         <v>2020</v>
       </c>
       <c r="D43" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E43" t="s">
-        <v>128</v>
+        <v>132</v>
+      </c>
+      <c r="F43" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H43" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B44">
         <v>2020</v>
       </c>
       <c r="D44" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="E44" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="F44" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="G44" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="B45">
         <v>2020</v>
       </c>
       <c r="D45" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="E45" t="s">
-        <v>132</v>
-      </c>
-      <c r="F45" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="G45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H45" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="B46">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D46" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E46" t="s">
-        <v>138</v>
-      </c>
-      <c r="F46" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="G46" t="s">
-        <v>140</v>
+        <v>148</v>
+      </c>
+      <c r="H46" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="B47">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D47" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="E47" t="s">
-        <v>143</v>
+        <v>152</v>
+      </c>
+      <c r="F47" t="s">
+        <v>153</v>
       </c>
       <c r="G47" t="s">
-        <v>144</v>
+        <v>153</v>
+      </c>
+      <c r="H47" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="B48">
         <v>2019</v>
       </c>
       <c r="D48" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="E48" t="s">
-        <v>147</v>
-      </c>
-      <c r="G48" t="s">
-        <v>148</v>
-      </c>
-      <c r="H48" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B49">
         <v>2019</v>
       </c>
       <c r="D49" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="E49" t="s">
-        <v>152</v>
-      </c>
-      <c r="F49" t="s">
-        <v>153</v>
-      </c>
-      <c r="G49" t="s">
-        <v>153</v>
-      </c>
-      <c r="H49" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B50">
         <v>2019</v>
       </c>
       <c r="D50" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="E50" t="s">
-        <v>157</v>
+        <v>163</v>
+      </c>
+      <c r="G50" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B51">
         <v>2019</v>
       </c>
       <c r="D51" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="E51" t="s">
-        <v>160</v>
+        <v>167</v>
+      </c>
+      <c r="F51" t="s">
+        <v>168</v>
+      </c>
+      <c r="G51" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B52">
         <v>2019</v>
       </c>
       <c r="D52" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="E52" t="s">
-        <v>163</v>
+        <v>171</v>
+      </c>
+      <c r="F52" t="s">
+        <v>172</v>
       </c>
       <c r="G52" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B53">
         <v>2019</v>
       </c>
       <c r="D53" t="s">
-        <v>166</v>
-      </c>
-      <c r="E53" t="s">
-        <v>167</v>
-      </c>
-      <c r="F53" t="s">
-        <v>168</v>
-      </c>
-      <c r="G53" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B54">
         <v>2019</v>
       </c>
       <c r="D54" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="E54" t="s">
-        <v>171</v>
-      </c>
-      <c r="F54" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="G54" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B55">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D55" t="s">
-        <v>174</v>
+        <v>180</v>
+      </c>
+      <c r="E55" t="s">
+        <v>181</v>
+      </c>
+      <c r="F55" t="s">
+        <v>182</v>
+      </c>
+      <c r="G55" t="s">
+        <v>182</v>
+      </c>
+      <c r="H55" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="B56">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D56" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="E56" t="s">
-        <v>177</v>
+        <v>186</v>
+      </c>
+      <c r="F56" t="s">
+        <v>187</v>
       </c>
       <c r="G56" t="s">
-        <v>178</v>
+        <v>187</v>
+      </c>
+      <c r="H56" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="B57">
         <v>2018</v>
       </c>
       <c r="D57" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="E57" t="s">
-        <v>181</v>
-      </c>
-      <c r="F57" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="G57" t="s">
-        <v>182</v>
-      </c>
-      <c r="H57" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="B58">
         <v>2018</v>
       </c>
       <c r="D58" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="E58" t="s">
-        <v>186</v>
-      </c>
-      <c r="F58" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="G58" t="s">
-        <v>187</v>
-      </c>
-      <c r="H58" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B59">
         <v>2018</v>
       </c>
       <c r="D59" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="E59" t="s">
-        <v>191</v>
+        <v>199</v>
+      </c>
+      <c r="F59" t="s">
+        <v>200</v>
       </c>
       <c r="G59" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B60">
         <v>2018</v>
       </c>
       <c r="D60" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="E60" t="s">
-        <v>195</v>
+        <v>203</v>
+      </c>
+      <c r="F60" t="s">
+        <v>204</v>
       </c>
       <c r="G60" t="s">
-        <v>196</v>
+        <v>205</v>
+      </c>
+      <c r="H60" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="B61">
         <v>2018</v>
       </c>
       <c r="D61" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="E61" t="s">
-        <v>199</v>
-      </c>
-      <c r="F61" t="s">
-        <v>200</v>
-      </c>
-      <c r="G61" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B62">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D62" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="E62" t="s">
-        <v>203</v>
-      </c>
-      <c r="F62" t="s">
-        <v>204</v>
-      </c>
-      <c r="G62" t="s">
-        <v>205</v>
-      </c>
-      <c r="H62" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B63">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D63" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="E63" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B64">
         <v>2017</v>
       </c>
       <c r="D64" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="E64" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B65">
         <v>2017</v>
       </c>
       <c r="D65" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="E65" t="s">
-        <v>215</v>
+        <v>221</v>
+      </c>
+      <c r="F65" t="s">
+        <v>222</v>
+      </c>
+      <c r="G65" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="B66">
         <v>2017</v>
       </c>
       <c r="D66" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="E66" t="s">
-        <v>218</v>
+        <v>225</v>
+      </c>
+      <c r="G66" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B67">
         <v>2017</v>
       </c>
       <c r="D67" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="E67" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="F67" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="G67" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="B68">
         <v>2017</v>
       </c>
       <c r="D68" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="E68" t="s">
-        <v>225</v>
-      </c>
-      <c r="G68" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="B69">
-        <v>2017</v>
+        <v>2016</v>
+      </c>
+      <c r="C69" t="s">
+        <v>306</v>
       </c>
       <c r="D69" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="E69" t="s">
-        <v>229</v>
-      </c>
-      <c r="F69" t="s">
-        <v>230</v>
-      </c>
-      <c r="G69" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B70">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D70" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E70" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B71">
         <v>2016</v>
       </c>
-      <c r="C71" t="s">
-        <v>306</v>
-      </c>
       <c r="D71" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="E71" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B72">
         <v>2016</v>
       </c>
       <c r="D72" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="E72" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B73">
         <v>2016</v>
       </c>
       <c r="D73" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="E73" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B74">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D74" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="E74" t="s">
-        <v>244</v>
+        <v>250</v>
+      </c>
+      <c r="G74" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="B75">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D75" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="E75" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="B76">
         <v>2015</v>
       </c>
       <c r="D76" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="E76" t="s">
-        <v>250</v>
-      </c>
-      <c r="G76" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B77">
         <v>2015</v>
       </c>
       <c r="D77" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="E77" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="B78">
         <v>2015</v>
       </c>
       <c r="D78" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="E78" t="s">
-        <v>257</v>
+        <v>263</v>
+      </c>
+      <c r="G78" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="B79">
         <v>2015</v>
       </c>
       <c r="D79" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="E79" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="B80">
         <v>2015</v>
       </c>
       <c r="D80" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="E80" t="s">
-        <v>263</v>
-      </c>
-      <c r="G80" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="B81">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D81" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="E81" t="s">
-        <v>267</v>
+        <v>273</v>
+      </c>
+      <c r="F81" t="s">
+        <v>274</v>
+      </c>
+      <c r="G81" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="B82">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D82" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="E82" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="B83">
         <v>2014</v>
       </c>
       <c r="D83" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="E83" t="s">
-        <v>273</v>
-      </c>
-      <c r="F83" t="s">
-        <v>274</v>
-      </c>
-      <c r="G83" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="B84">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D84" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="E84" t="s">
-        <v>277</v>
+        <v>283</v>
+      </c>
+      <c r="G84" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="B85">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="D85" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="E85" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="B86">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="D86" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="E86" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="G86" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="B87">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D87" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="E87" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="B88">
         <v>2011</v>
       </c>
       <c r="D88" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="E88" t="s">
-        <v>290</v>
-      </c>
-      <c r="G88" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="B89">
         <v>2011</v>
       </c>
       <c r="D89" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="E89" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="B90">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="D90" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="E90" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>298</v>
-      </c>
-      <c r="B91">
-        <v>2011</v>
-      </c>
-      <c r="D91" t="s">
-        <v>299</v>
-      </c>
-      <c r="E91" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>301</v>
-      </c>
-      <c r="B92">
-        <v>2010</v>
-      </c>
-      <c r="D92" t="s">
-        <v>302</v>
-      </c>
-      <c r="E92" t="s">
         <v>303</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="F10" r:id="rId1" xr:uid="{57E6435F-936F-B049-820C-8B8D8672A77C}"/>
+    <hyperlink ref="F8" r:id="rId1" xr:uid="{57E6435F-936F-B049-820C-8B8D8672A77C}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{38F66897-270C-C042-88B5-0D5A01D7EACC}"/>
+    <hyperlink ref="A22" r:id="rId3" xr:uid="{B55B63E9-0A94-FA45-BAFB-9E370BC2303E}"/>
+    <hyperlink ref="A3" r:id="rId4" display="https://psycnet.apa.org/doi/10.1037/emo0001508" xr:uid="{EEC9F15A-C0E6-7D4A-AC67-31429CF8D170}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2899,8 +2918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692218B6-AC24-C04C-84F2-434F3CE1F2AE}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>